<commit_message>
Burndownchart med korrekte estimeringer o.a.
</commit_message>
<xml_diff>
--- a/Diagrammer/Burndown for WHAT.xlsx
+++ b/Diagrammer/Burndown for WHAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\GitHub Repositorys\3-sem.-eksamen-SWD\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69FB32B-4584-438B-A8A2-99C52F875777}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA249011-5346-4292-BBAB-A8FE179474E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
+    <workbookView xWindow="4185" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Est.</t>
   </si>
@@ -48,9 +48,6 @@
     <t>US1.02</t>
   </si>
   <si>
-    <t>US1.03</t>
-  </si>
-  <si>
     <t>US1.04</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t>US2.01</t>
-  </si>
-  <si>
-    <t>US2.02</t>
   </si>
   <si>
     <t>US2.03</t>
@@ -156,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -164,13 +158,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -308,22 +387,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1860</c:v>
+                  <c:v>1530</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1550</c:v>
+                  <c:v>1275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1240</c:v>
+                  <c:v>1020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>930</c:v>
+                  <c:v>765</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>620</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>310</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -383,13 +462,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1860</c:v>
+                  <c:v>1530</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1800</c:v>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1560</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1260,15 +1339,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1594,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748780FD-D025-4A00-ABEB-C79BF8E25DEA}">
-  <dimension ref="B3:O30"/>
+  <dimension ref="B1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,44 +1684,54 @@
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L1">
+        <f>SUM(1530/6)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D4">
         <v>130</v>
@@ -1657,15 +1746,15 @@
       <c r="H4">
         <v>130</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="7">
         <v>0</v>
       </c>
-      <c r="K4">
-        <f>SUM(C4:C17)</f>
-        <v>1860</v>
-      </c>
-      <c r="L4">
-        <v>1860</v>
+      <c r="K4" s="8">
+        <f>SUM(C4:C15)</f>
+        <v>1530</v>
+      </c>
+      <c r="L4" s="9">
+        <v>1530</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -1676,7 +1765,7 @@
         <v>120</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1685,18 +1774,18 @@
         <v>240</v>
       </c>
       <c r="H5">
-        <v>130</v>
-      </c>
-      <c r="J5">
+        <v>140</v>
+      </c>
+      <c r="J5" s="7">
         <v>1</v>
       </c>
-      <c r="K5">
-        <f>SUM(K4-310)</f>
-        <v>1550</v>
-      </c>
-      <c r="L5">
+      <c r="K5" s="8">
+        <f>SUM(K4-255)</f>
+        <v>1275</v>
+      </c>
+      <c r="L5" s="9">
         <f>SUM(L4-C4)</f>
-        <v>1800</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -1707,21 +1796,21 @@
         <v>120</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="7">
         <v>2</v>
       </c>
-      <c r="K6">
-        <f t="shared" ref="K6:K10" si="0">SUM(K5-310)</f>
-        <v>1240</v>
-      </c>
-      <c r="L6">
+      <c r="K6" s="8">
+        <f t="shared" ref="K6:K10" si="0">SUM(K5-255)</f>
+        <v>1020</v>
+      </c>
+      <c r="L6" s="9">
         <f>SUM(L5-(C5+C6))</f>
-        <v>1560</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -1729,79 +1818,83 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="7">
         <v>3</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="8">
         <f t="shared" si="0"/>
-        <v>930</v>
-      </c>
+        <v>765</v>
+      </c>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="7">
         <v>4</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="8">
         <f t="shared" si="0"/>
-        <v>620</v>
-      </c>
+        <v>510</v>
+      </c>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="7">
         <v>5</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="8">
         <f t="shared" si="0"/>
-        <v>310</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>120</v>
+        <v>210</v>
       </c>
       <c r="F10">
         <v>7</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>6</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="F11">
         <v>8</v>
@@ -1812,7 +1905,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F12">
         <v>9</v>
@@ -1823,10 +1916,10 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -1837,7 +1930,7 @@
         <v>120</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -1845,10 +1938,10 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
@@ -1859,7 +1952,7 @@
         <v>180</v>
       </c>
       <c r="F16">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1870,7 +1963,7 @@
         <v>240</v>
       </c>
       <c r="F17">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1878,10 +1971,10 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>120</v>
+        <v>330</v>
       </c>
       <c r="F18">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1889,10 +1982,10 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="F19">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1900,10 +1993,10 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F20">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1911,10 +2004,10 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="F21">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1922,10 +2015,10 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F22">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -1933,10 +2026,7 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <v>60</v>
-      </c>
-      <c r="F23">
-        <v>20</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -1944,10 +2034,7 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <v>120</v>
-      </c>
-      <c r="F24">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -1955,7 +2042,7 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -1963,7 +2050,7 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <v>60</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -1971,33 +2058,18 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <v>120</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
       <c r="C28">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <f>SUM(C4:C29)/60</f>
-        <v>67</v>
+        <f>SUM(C4:C27)/60</f>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sprint review ½ done + udlæg til arbejdsplan
</commit_message>
<xml_diff>
--- a/Diagrammer/Burndown for WHAT.xlsx
+++ b/Diagrammer/Burndown for WHAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\GitHub Repositorys\3-sem.-eksamen-SWD\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8960CFD1-BBE2-44E1-AD90-D6902F2E9566}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D89B88-709C-4FE0-A053-865E4088F5B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
+    <workbookView xWindow="6045" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
                   <c:v>810</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1682,7 +1682,7 @@
   <dimension ref="B3:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,8 +1859,8 @@
         <v>510</v>
       </c>
       <c r="L8" s="9">
-        <f>SUM(L7-(C10+C11+C12+C13+C14))</f>
-        <v>180</v>
+        <f>SUM(L7-(C10+C11+C12+C13+C14+C15))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sprint review til review og opdateret Gantt-chart
</commit_message>
<xml_diff>
--- a/Diagrammer/Burndown for WHAT.xlsx
+++ b/Diagrammer/Burndown for WHAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\GitHub Repositorys\3-sem.-eksamen-SWD\Diagrammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D89B88-709C-4FE0-A053-865E4088F5B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CABE830-D5CF-45AF-A4F6-C338AA2A0D00}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
+    <workbookView xWindow="6975" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0E5311F3-3848-4F1F-B0A1-818DE07B362D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Est.</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Actual</t>
+  </si>
+  <si>
+    <t>I alt</t>
+  </si>
+  <si>
+    <t>timer</t>
+  </si>
+  <si>
+    <t>Resterende min</t>
   </si>
 </sst>
 </file>
@@ -150,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -235,11 +244,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -250,6 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,6 +401,36 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Ark1'!$J$4:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Ark1'!$K$4:$K$10</c:f>
@@ -455,6 +506,36 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Ark1'!$J$4:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Ark1'!$L$4:$L$10</c:f>
@@ -561,6 +642,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1345,16 +1427,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1679,14 +1761,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748780FD-D025-4A00-ABEB-C79BF8E25DEA}">
-  <dimension ref="B3:O28"/>
+  <dimension ref="B3:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1741,10 +1825,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H4">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="J4" s="7">
         <v>0</v>
@@ -1774,7 +1858,7 @@
         <v>240</v>
       </c>
       <c r="H5">
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="J5" s="7">
         <v>1</v>
@@ -1801,6 +1885,12 @@
       <c r="F6">
         <v>3</v>
       </c>
+      <c r="G6">
+        <v>510</v>
+      </c>
+      <c r="H6">
+        <v>510</v>
+      </c>
       <c r="J6" s="7">
         <v>2</v>
       </c>
@@ -2091,10 +2181,32 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C28">
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="10">
         <f>SUM(C4:C27)/60</f>
         <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f>SUM(62*60)-(C4+C5+C6+C7+C8+C9+C10+C11+C12+C13+C14)</f>
+        <v>2370</v>
+      </c>
+      <c r="C31">
+        <f>SUM(B31/60)</f>
+        <v>39.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>